<commit_message>
bf: update lf lf tas form
</commit_message>
<xml_diff>
--- a/LF/TAS/Burkina Faso/2023/september/bf_lf_tas1_202309_1_site.xlsx
+++ b/LF/TAS/Burkina Faso/2023/september/bf_lf_tas1_202309_1_site.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Burkina Faso\2023\september\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DDCD86-59F4-4670-A11B-83F91E0A976A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BC04E9-3156-4ECB-88D3-BD3664CE922B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="359">
   <si>
     <t>form_title</t>
   </si>
@@ -1113,6 +1113,9 @@
   </si>
   <si>
     <t>Site Code</t>
+  </si>
+  <si>
+    <t>N.TONHERO</t>
   </si>
 </sst>
 </file>
@@ -1427,17 +1430,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2097,8 +2090,8 @@
   <dimension ref="A1:H255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A256" sqref="A256:XFD337"/>
+      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" activeCellId="1" sqref="B1:B1048576 D1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4060,7 +4053,7 @@
         <v>73</v>
       </c>
       <c r="B146" t="s">
-        <v>204</v>
+        <v>358</v>
       </c>
       <c r="C146" t="s">
         <v>204</v>
@@ -5343,7 +5336,7 @@
         <v>107</v>
       </c>
       <c r="H238" t="s">
-        <v>204</v>
+        <v>358</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.25">
@@ -5651,7 +5644,7 @@
   <dimension ref="A1:U85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2:F85"/>
     </sheetView>
   </sheetViews>

</xml_diff>